<commit_message>
Excel data provider code completed.
</commit_message>
<xml_diff>
--- a/input-files/TestData2.xlsx
+++ b/input-files/TestData2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahesh\git\repository\SeleniumTraining\input-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF02291-2674-42E1-AEE9-BF46070CA35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DE09F9-C2A4-48DD-B142-05F8E8C2A3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C8EDC8FC-EF1D-4EAC-9FD6-5E82640E3E93}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>